<commit_message>
falta Kg e calcular os finais
</commit_message>
<xml_diff>
--- a/entrada.xlsx
+++ b/entrada.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayra Peter\Documents\5 SEMESTRE\Transferencia de Calor e Mecanica dos Solidos\TermoSol1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB642D65-9D4B-43A3-BB16-CB1A0DE3E3D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="130" windowWidth="21060" windowHeight="10840" activeTab="3"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nos" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,17 @@
     <sheet name="Carregamento" sheetId="3" r:id="rId3"/>
     <sheet name="Restricao" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -61,8 +77,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +88,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -120,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -152,6 +176,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -162,12 +190,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -209,7 +240,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -242,9 +273,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -277,6 +325,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -452,11 +517,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -478,40 +543,83 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="9">
-        <f>COUNT(A2:A1048576)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
+        <v>-2</v>
+      </c>
+      <c r="B3" s="2">
         <v>0</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.4</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="B4" s="2">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="10">
+        <v>2</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="10">
+        <v>-2</v>
+      </c>
+      <c r="B7" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="10">
+        <v>0</v>
+      </c>
+      <c r="B8" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="10">
+        <v>2</v>
+      </c>
+      <c r="B9" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="10">
+        <v>0</v>
+      </c>
+      <c r="B10" s="10">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -519,11 +627,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -560,12 +668,11 @@
         <v>210000000000</v>
       </c>
       <c r="D2" s="3">
-        <v>2.0000000000000001E-4</v>
+        <v>7.0685799999999993E-2</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="7">
-        <f>COUNT(A2:A1048576)</f>
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -579,24 +686,207 @@
         <v>210000000000</v>
       </c>
       <c r="D3" s="3">
-        <v>2.0000000000000001E-4</v>
+        <v>7.0685799999999993E-2</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D4" s="3">
+        <v>7.0685799999999993E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D5" s="3">
+        <v>7.0685799999999993E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="3">
-        <v>210000000000</v>
-      </c>
-      <c r="D4" s="3">
-        <v>2.0000000000000001E-4</v>
+      <c r="B6" s="2">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D6" s="3">
+        <v>7.0685799999999993E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D7" s="3">
+        <v>7.0685799999999993E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D8" s="3">
+        <v>7.0685799999999993E-2</v>
+      </c>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D9" s="3">
+        <v>7.0685799999999993E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D10" s="3">
+        <v>7.0685799999999993E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D11" s="3">
+        <v>7.0685799999999993E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D12" s="3">
+        <v>7.0685799999999993E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D13" s="3">
+        <v>7.0685799999999993E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D14" s="3">
+        <v>7.0685799999999993E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2">
+        <v>9</v>
+      </c>
+      <c r="C15" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D15" s="3">
+        <v>7.0685799999999993E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D16" s="3">
+        <v>7.0685799999999993E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>8</v>
+      </c>
+      <c r="B17" s="2">
+        <v>9</v>
+      </c>
+      <c r="C17" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D17" s="3">
+        <v>7.0685799999999993E-2</v>
       </c>
     </row>
   </sheetData>
@@ -606,11 +896,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -635,37 +925,42 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>150</v>
+        <v>4000</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="9">
-        <f>COUNT(A2:A1048576)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2">
-        <v>-100</v>
+        <v>4000</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="2">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>20000</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
@@ -808,11 +1103,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -841,16 +1136,15 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="9">
-        <f>COUNT(A2:A1048576)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -866,29 +1160,47 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10">
+        <v>2</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>

</xml_diff>